<commit_message>
added fb msg status
</commit_message>
<xml_diff>
--- a/app-design/bank discounts/Banks List.xlsx
+++ b/app-design/bank discounts/Banks List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Askari Bank</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>no email</t>
+  </si>
+  <si>
+    <t>FB Msg</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +192,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -232,6 +241,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -534,21 +550,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -559,10 +576,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -573,11 +593,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -588,11 +609,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -603,11 +625,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -618,11 +641,12 @@
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -632,11 +656,14 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -646,11 +673,14 @@
       <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -661,11 +691,12 @@
         <v>1</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -675,11 +706,14 @@
       <c r="C9" s="3">
         <v>0</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -690,11 +724,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -704,34 +739,38 @@
       <c r="C11" s="3">
         <v>0</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="9">
         <v>0</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -741,14 +780,17 @@
       <c r="C13" s="3">
         <v>0</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -759,11 +801,12 @@
         <v>1</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -773,14 +816,15 @@
       <c r="C15" s="3">
         <v>0</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -791,11 +835,12 @@
         <v>1</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -806,11 +851,12 @@
         <v>1</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -821,7 +867,8 @@
         <v>1</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -832,26 +879,26 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="E8" r:id="rId5"/>
-    <hyperlink ref="E10" r:id="rId6"/>
-    <hyperlink ref="E11" r:id="rId7"/>
-    <hyperlink ref="E12" r:id="rId8"/>
-    <hyperlink ref="E13" r:id="rId9"/>
-    <hyperlink ref="E14" r:id="rId10"/>
-    <hyperlink ref="E15" r:id="rId11"/>
-    <hyperlink ref="E16" r:id="rId12"/>
-    <hyperlink ref="E17" r:id="rId13"/>
-    <hyperlink ref="E18" r:id="rId14"/>
-    <hyperlink ref="D15" r:id="rId15"/>
-    <hyperlink ref="D12" r:id="rId16"/>
-    <hyperlink ref="D13" r:id="rId17"/>
-    <hyperlink ref="D11" r:id="rId18"/>
-    <hyperlink ref="D7" r:id="rId19"/>
-    <hyperlink ref="D6" r:id="rId20"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId4"/>
+    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="F10" r:id="rId6"/>
+    <hyperlink ref="F11" r:id="rId7"/>
+    <hyperlink ref="F12" r:id="rId8"/>
+    <hyperlink ref="F13" r:id="rId9"/>
+    <hyperlink ref="F14" r:id="rId10"/>
+    <hyperlink ref="F15" r:id="rId11"/>
+    <hyperlink ref="F16" r:id="rId12"/>
+    <hyperlink ref="F17" r:id="rId13"/>
+    <hyperlink ref="F18" r:id="rId14"/>
+    <hyperlink ref="E15" r:id="rId15"/>
+    <hyperlink ref="E12" r:id="rId16"/>
+    <hyperlink ref="E13" r:id="rId17"/>
+    <hyperlink ref="E11" r:id="rId18"/>
+    <hyperlink ref="E7" r:id="rId19"/>
+    <hyperlink ref="E6" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId21"/>

</xml_diff>

<commit_message>
fixed: deals in alphabetical order
</commit_message>
<xml_diff>
--- a/app-design/bank discounts/Banks List.xlsx
+++ b/app-design/bank discounts/Banks List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,12 +192,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -241,7 +235,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,7 +243,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -312,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -347,7 +339,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -559,7 +551,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,21 +666,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="9">
         <v>0</v>
       </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>36</v>
       </c>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -707,22 +700,22 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>0</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>0</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -741,59 +734,59 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="9">
         <v>0</v>
       </c>
-      <c r="D11" s="8">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="12"/>
       <c r="G11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>0</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>0</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>0</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -815,17 +808,17 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="9">
         <v>0</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="12" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed: disable deal, wip: add deal without pic
</commit_message>
<xml_diff>
--- a/app-design/bank discounts/Banks List.xlsx
+++ b/app-design/bank discounts/Banks List.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$E$18</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Askari Bank</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>https://www.facebook.com/pg/SoneriBankPK/photos/?tab=album&amp;album_id=560208060705453</t>
+  </si>
+  <si>
+    <t>Bank Uploaded</t>
   </si>
 </sst>
 </file>
@@ -548,23 +551,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -572,329 +577,367 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <v>0</v>
       </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="4" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
         <v>0</v>
       </c>
-      <c r="D9" s="10">
+      <c r="F9" s="10">
         <v>0</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
         <v>0</v>
       </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" t="s">
+      <c r="H11" s="12"/>
+      <c r="I11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
         <v>0</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
         <v>0</v>
       </c>
-      <c r="D13" s="10">
+      <c r="F13" s="10">
         <v>0</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="4" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9">
         <v>0</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="H15" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="4" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="4" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="4" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C18">
+  <autoFilter ref="B1:E18">
     <sortState ref="B2:C18">
       <sortCondition ref="B1:B18"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F2" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="F10" r:id="rId6"/>
-    <hyperlink ref="F14" r:id="rId7"/>
-    <hyperlink ref="F16" r:id="rId8"/>
-    <hyperlink ref="F17" r:id="rId9"/>
-    <hyperlink ref="F18" r:id="rId10"/>
-    <hyperlink ref="E15" r:id="rId11"/>
-    <hyperlink ref="E12" r:id="rId12"/>
-    <hyperlink ref="E13" r:id="rId13"/>
-    <hyperlink ref="E11" r:id="rId14"/>
-    <hyperlink ref="E7" r:id="rId15"/>
-    <hyperlink ref="E6" r:id="rId16"/>
-    <hyperlink ref="F6" r:id="rId17"/>
-    <hyperlink ref="F15" r:id="rId18"/>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H5" r:id="rId3"/>
+    <hyperlink ref="H2" r:id="rId4"/>
+    <hyperlink ref="H8" r:id="rId5"/>
+    <hyperlink ref="H10" r:id="rId6"/>
+    <hyperlink ref="H14" r:id="rId7"/>
+    <hyperlink ref="H16" r:id="rId8"/>
+    <hyperlink ref="H17" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="G15" r:id="rId11"/>
+    <hyperlink ref="G12" r:id="rId12"/>
+    <hyperlink ref="G13" r:id="rId13"/>
+    <hyperlink ref="G11" r:id="rId14"/>
+    <hyperlink ref="G7" r:id="rId15"/>
+    <hyperlink ref="G6" r:id="rId16"/>
+    <hyperlink ref="H6" r:id="rId17"/>
+    <hyperlink ref="H15" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>

</xml_diff>